<commit_message>
t'es rendu a suggererCorrection et tu vas devoir tester _supprimerAVL
</commit_message>
<xml_diff>
--- a/NoteTp3-IFT2008.xlsx
+++ b/NoteTp3-IFT2008.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t xml:space="preserve">Correction TP3: Ajoutez s.v.p. ici votre nom et matricule</t>
   </si>
@@ -54,10 +54,10 @@
     <t xml:space="preserve">void ajouteMot(const std ::string&amp; motOriginal, const std ::string&amp; motTraduit);</t>
   </si>
   <si>
-    <t xml:space="preserve">Tes entrain de faire ca</t>
-  </si>
-  <si>
     <t xml:space="preserve">void supprimeMot(const std ::string&amp; motOriginal);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK, mais reste a tester si vecteur / string se delete comme il le faut</t>
   </si>
   <si>
     <t xml:space="preserve">double similitude(const std ::string&amp; mot1, const std ::string&amp; mot2);</t>
@@ -238,7 +238,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -264,10 +264,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -307,10 +303,10 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.29"/>
@@ -421,12 +417,12 @@
         <v>14</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I7" s="7" t="n">
         <v>14</v>
@@ -436,6 +432,9 @@
       </c>
       <c r="K7" s="7" t="n">
         <v>14</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -668,7 +667,7 @@
       <c r="I22" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K22" s="7" t="n">
@@ -688,7 +687,7 @@
       <c r="K23" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="L23" s="9"/>
+      <c r="L23" s="8"/>
     </row>
     <row r="24" s="3" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
@@ -741,7 +740,7 @@
       <c r="H28" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I28" s="10" t="n">
+      <c r="I28" s="9" t="n">
         <f aca="false">SUM(I3,I14,I19)</f>
         <v>100</v>
       </c>
@@ -754,14 +753,14 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -788,7 +787,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -811,7 +810,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>